<commit_message>
Reject payment done, employee error fixed
</commit_message>
<xml_diff>
--- a/public/employees.xlsx
+++ b/public/employees.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shehu.abdullahi\Documents\Apps\Edsine\ebslive\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0976B8C8-2136-8241-95DF-070BBE99D8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21220" yWindow="0" windowWidth="14620" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21216" yWindow="0" windowWidth="14616" windowHeight="22404"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
@@ -91,9 +90,6 @@
     <t>dependants_number</t>
   </si>
   <si>
-    <t>monthly_remuneration</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -134,12 +130,15 @@
   </si>
   <si>
     <t>ADEMOLA SHOLA</t>
+  </si>
+  <si>
+    <t>monthly_renumeration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-m\-d"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
@@ -979,20 +978,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -1000,7 +999,7 @@
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,36 +1070,36 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1004033022</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
       </c>
       <c r="F2" s="2">
         <v>43868</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
       </c>
       <c r="I2">
         <v>1234</v>
@@ -1109,19 +1108,19 @@
         <v>44686</v>
       </c>
       <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
-        <v>34</v>
-      </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2">
         <v>80444534423</v>
@@ -1130,16 +1129,16 @@
         <v>8654322190</v>
       </c>
       <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
         <v>35</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s">
         <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" t="s">
-        <v>37</v>
       </c>
       <c r="V2">
         <v>9066656643</v>
@@ -1154,30 +1153,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1004033022</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="2">
         <v>43869</v>
       </c>
       <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
         <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
       </c>
       <c r="I3">
         <v>5643</v>
@@ -1186,19 +1185,19 @@
         <v>44656</v>
       </c>
       <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3">
         <v>80444534423</v>
@@ -1207,16 +1206,16 @@
         <v>8654322190</v>
       </c>
       <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
         <v>35</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
         <v>36</v>
-      </c>
-      <c r="T3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" t="s">
-        <v>37</v>
       </c>
       <c r="V3">
         <v>9066656643</v>
@@ -1231,13 +1230,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="F6" s="2"/>
     </row>
   </sheetData>

</xml_diff>